<commit_message>
day 28 write into excel
</commit_message>
<xml_diff>
--- a/VytrackTestUsers.xlsx
+++ b/VytrackTestUsers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marufjon/IdeaProjects/va-spring-2019-selenium-testng/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alisazakirova/IdeaProjects/Fall2019Selenium_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDDC9C1-934F-044B-80DB-58DA20C1AFF6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AB3E6B-7869-E64D-8575-9039343D9BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41120" yWindow="1540" windowWidth="33600" windowHeight="18920" activeTab="5" xr2:uid="{506372D9-39D2-EA47-AA3D-ABD5428ED2AB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="5" xr2:uid="{506372D9-39D2-EA47-AA3D-ABD5428ED2AB}"/>
   </bookViews>
   <sheets>
     <sheet name="QA1-all" sheetId="4" r:id="rId1"/>
@@ -4829,8 +4829,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -9073,8 +9073,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -9413,7 +9413,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -13660,7 +13660,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -13999,7 +13999,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -18240,13 +18240,13 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -18266,7 +18266,7 @@
         <v>303</v>
       </c>
       <c r="F1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
day 28 Login test with excel file
</commit_message>
<xml_diff>
--- a/VytrackTestUsers.xlsx
+++ b/VytrackTestUsers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alisazakirova/IdeaProjects/Fall2019Selenium_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marufjon/IdeaProjects/va-spring-2019-selenium-testng/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AB3E6B-7869-E64D-8575-9039343D9BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDDC9C1-934F-044B-80DB-58DA20C1AFF6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="5" xr2:uid="{506372D9-39D2-EA47-AA3D-ABD5428ED2AB}"/>
+    <workbookView xWindow="41120" yWindow="1540" windowWidth="33600" windowHeight="18920" activeTab="5" xr2:uid="{506372D9-39D2-EA47-AA3D-ABD5428ED2AB}"/>
   </bookViews>
   <sheets>
     <sheet name="QA1-all" sheetId="4" r:id="rId1"/>
@@ -4829,8 +4829,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -9073,8 +9073,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -9413,7 +9413,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -13660,7 +13660,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -13999,7 +13999,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -18240,13 +18240,13 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -18266,7 +18266,7 @@
         <v>303</v>
       </c>
       <c r="F1" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>